<commit_message>
add penalty factor for delay in objective function
</commit_message>
<xml_diff>
--- a/Delay Model/data.xlsx
+++ b/Delay Model/data.xlsx
@@ -386,16 +386,16 @@
         <v>0</v>
       </c>
       <c r="C1">
-        <v>3365.7963823295108</v>
+        <v>3437.9810620581961</v>
       </c>
       <c r="D1">
-        <v>3365.7963823295108</v>
+        <v>3437.9810620581961</v>
       </c>
       <c r="E1">
-        <v>3365.7963823295108</v>
+        <v>3437.9810620581961</v>
       </c>
       <c r="F1">
-        <v>3365.7963823295108</v>
+        <v>3437.9810620581961</v>
       </c>
       <c r="G1">
         <v>12000</v>
@@ -422,16 +422,16 @@
         <v>0</v>
       </c>
       <c r="O1">
-        <v>1.1757891266621858</v>
+        <v>2.1722486486763244</v>
       </c>
       <c r="P1">
-        <v>4.4086019364397875E-3</v>
+        <v>4.2911264477147317E-3</v>
       </c>
       <c r="Q1">
-        <v>4.3645130726325627E-3</v>
+        <v>4.0177754921099425E-3</v>
       </c>
       <c r="R1">
-        <v>3.7198960526813565</v>
+        <v>3.6928380058521566</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
@@ -442,16 +442,16 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>7846.4664574118069</v>
+        <v>7963.3709603826101</v>
       </c>
       <c r="D2">
-        <v>15365.79638232951</v>
+        <v>16639.936190263325</v>
       </c>
       <c r="E2">
-        <v>7846.4664574118069</v>
+        <v>7963.3709603826101</v>
       </c>
       <c r="F2">
-        <v>7846.4664574118069</v>
+        <v>7963.3709603826101</v>
       </c>
       <c r="G2">
         <v>24000</v>
@@ -478,16 +478,16 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>3.5266895492610564</v>
+        <v>6.7413431515914519</v>
       </c>
       <c r="P2">
-        <v>7.2661291997131667E-3</v>
+        <v>8.793026108856258E-3</v>
       </c>
       <c r="Q2">
-        <v>7.8600488618388691E-3</v>
+        <v>7.9652932464109524E-3</v>
       </c>
       <c r="R2">
-        <v>2.127070932155203</v>
+        <v>2.0414773808484235</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -498,16 +498,16 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>15576.765678430065</v>
+        <v>15719.502686049842</v>
       </c>
       <c r="D3">
-        <v>23096.095603347771</v>
+        <v>24396.067915930555</v>
       </c>
       <c r="E3">
-        <v>15576.765678430065</v>
+        <v>15719.502686049842</v>
       </c>
       <c r="F3">
-        <v>15576.765678430065</v>
+        <v>15719.502686049842</v>
       </c>
       <c r="G3">
         <v>36000</v>
@@ -534,16 +534,16 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>9.3555172377501936</v>
+        <v>9.4478216830169988</v>
       </c>
       <c r="P3">
-        <v>1.0338696340652749E-2</v>
+        <v>1.1140260329096346E-2</v>
       </c>
       <c r="Q3">
-        <v>1.0837327168098322E-2</v>
+        <v>1.151572678216432E-2</v>
       </c>
       <c r="R3">
-        <v>1.5068236761180864</v>
+        <v>1.4896000059164411</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -554,16 +554,16 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>23841.462561133318</v>
+        <v>23997.701653556047</v>
       </c>
       <c r="D4">
-        <v>31381.680013939927</v>
+        <v>33173.201411883587</v>
       </c>
       <c r="E4">
-        <v>23862.35008902222</v>
+        <v>24494.893075858083</v>
       </c>
       <c r="F4">
-        <v>23862.35008902222</v>
+        <v>24341.823999796783</v>
       </c>
       <c r="G4">
         <v>48000</v>
@@ -581,7 +581,7 @@
         <v>30.047657188626353</v>
       </c>
       <c r="L4">
-        <v>30.047657188626353</v>
+        <v>30.029244321927248</v>
       </c>
       <c r="M4">
         <v>40</v>
@@ -590,16 +590,16 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>11.105049255794201</v>
+        <v>11.141239101872866</v>
       </c>
       <c r="P4">
-        <v>1.4463707327313165E-2</v>
+        <v>1.5376489030264019E-2</v>
       </c>
       <c r="Q4">
-        <v>1.4627831678389089E-2</v>
+        <v>1.5269253535713545E-2</v>
       </c>
       <c r="R4">
-        <v>1.4606481290535087</v>
+        <v>0.3153986472398807</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
@@ -610,16 +610,16 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>30484.95053411361</v>
+        <v>30653.911403578168</v>
       </c>
       <c r="D5">
-        <v>38019.301346671884</v>
+        <v>39821.624078848217</v>
       </c>
       <c r="E5">
-        <v>30499.971421754177</v>
+        <v>31143.31574282272</v>
       </c>
       <c r="F5">
-        <v>30499.971421754177</v>
+        <v>31020.111972763196</v>
       </c>
       <c r="G5">
         <v>60000</v>
@@ -637,7 +637,7 @@
         <v>35.047657188626353</v>
       </c>
       <c r="L5">
-        <v>35.047657188626353</v>
+        <v>35.042217294900226</v>
       </c>
       <c r="M5">
         <v>45</v>
@@ -646,16 +646,16 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>11.021150707967598</v>
+        <v>13.07890057733656</v>
       </c>
       <c r="P5">
-        <v>1.7560736676558691E-2</v>
+        <v>1.9141677999400961E-2</v>
       </c>
       <c r="Q5">
-        <v>1.7359919013023851E-2</v>
+        <v>1.8657838274652002E-2</v>
       </c>
       <c r="R5">
-        <v>1.3893174674105073</v>
+        <v>0.2080766816274878</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -666,16 +666,16 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>36108.653193873208</v>
+        <v>36296.511994511246</v>
       </c>
       <c r="D6">
-        <v>43643.004006431482</v>
+        <v>45464.224669781288</v>
       </c>
       <c r="E6">
-        <v>36123.674081513775</v>
+        <v>36785.916333755798</v>
       </c>
       <c r="F6">
-        <v>36123.674081513775</v>
+        <v>36473.054073267122</v>
       </c>
       <c r="G6">
         <v>72000</v>
@@ -702,16 +702,16 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>11.537445240920041</v>
+        <v>13.023724075392526</v>
       </c>
       <c r="P6">
-        <v>2.1133072422074354E-2</v>
+        <v>2.1469854452705023E-2</v>
       </c>
       <c r="Q6">
-        <v>2.1081019118353569E-2</v>
+        <v>2.2541924953927137E-2</v>
       </c>
       <c r="R6">
-        <v>0.87519921766444508</v>
+        <v>0.13485645661499357</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
@@ -722,16 +722,16 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>43250.826101225575</v>
+        <v>43452.204522691391</v>
       </c>
       <c r="D7">
-        <v>50747.766999544096</v>
+        <v>55004.535550839893</v>
       </c>
       <c r="E7">
-        <v>43227.306619564028</v>
+        <v>45118.620898540736</v>
       </c>
       <c r="F7">
-        <v>43903.529384666501</v>
+        <v>44104.757740425368</v>
       </c>
       <c r="G7">
         <v>84000</v>
@@ -758,16 +758,16 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>9.1455370549833646</v>
+        <v>10.622044375014756</v>
       </c>
       <c r="P7">
-        <v>2.6902171362320291E-2</v>
+        <v>2.6266153946365754E-2</v>
       </c>
       <c r="Q7">
-        <v>2.4886883619906208E-2</v>
+        <v>2.5322936705173785E-2</v>
       </c>
       <c r="R7">
-        <v>0.92245536855872368</v>
+        <v>0.87471082683117407</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
@@ -778,16 +778,16 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>50314.148862493443</v>
+        <v>50546.618019861751</v>
       </c>
       <c r="D8">
-        <v>62659.036121223719</v>
+        <v>69383.614656866615</v>
       </c>
       <c r="E8">
-        <v>50276.981427243401</v>
+        <v>52215.720319221444</v>
       </c>
       <c r="F8">
-        <v>51028.355335040673</v>
+        <v>51717.348890623864</v>
       </c>
       <c r="G8">
         <v>96000</v>
@@ -814,16 +814,16 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>11.207010300011918</v>
+        <v>18.145465943912708</v>
       </c>
       <c r="P8">
-        <v>2.8927699098908959E-2</v>
+        <v>2.8420534942984566E-2</v>
       </c>
       <c r="Q8">
-        <v>2.9367165515568061E-2</v>
+        <v>2.8869103576687743E-2</v>
       </c>
       <c r="R8">
-        <v>4.7431906172071159</v>
+        <v>4.4307353994038614</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
@@ -834,16 +834,16 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>53457.510894370018</v>
+        <v>53755.358450139349</v>
       </c>
       <c r="D9">
-        <v>65736.409883952641</v>
+        <v>72477.823865821629</v>
       </c>
       <c r="E9">
-        <v>53435.364346760543</v>
+        <v>55749.287937245586</v>
       </c>
       <c r="F9">
-        <v>53727.274363764751</v>
+        <v>54774.9327272722</v>
       </c>
       <c r="G9">
         <v>108000</v>
@@ -852,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>55.029244321927251</v>
+        <v>55.047657188626353</v>
       </c>
       <c r="J9">
         <v>115</v>
@@ -870,16 +870,16 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>14.544679796804383</v>
+        <v>27.766133324155266</v>
       </c>
       <c r="P9">
-        <v>3.3966629565650733E-2</v>
+        <v>3.1925172949234942E-2</v>
       </c>
       <c r="Q9">
-        <v>3.3698967495698492E-2</v>
+        <v>3.2136515051226992E-2</v>
       </c>
       <c r="R9">
-        <v>0.19690968353582447</v>
+        <v>0.18635708509463603</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
@@ -890,16 +890,16 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>59359.252386211381</v>
+        <v>59726.204735787484</v>
       </c>
       <c r="D10">
-        <v>77736.409883952641</v>
+        <v>87477.823865821629</v>
       </c>
       <c r="E10">
-        <v>59385.625283790883</v>
+        <v>62895.591850531062</v>
       </c>
       <c r="F10">
-        <v>59536.048269731713</v>
+        <v>60377.114926591887</v>
       </c>
       <c r="G10">
         <v>120000</v>
@@ -926,72 +926,72 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>131.26149474901632</v>
+        <v>160.7193877507483</v>
       </c>
       <c r="P10">
-        <v>3.5259144385908971E-2</v>
+        <v>3.6029988391828825E-2</v>
       </c>
       <c r="Q10">
-        <v>3.6748494649745264E-2</v>
+        <v>3.563005973045491E-2</v>
       </c>
       <c r="R10">
-        <v>0.10929970670950018</v>
+        <v>0.10741697000279039</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11">
-        <v>64176.78174056342</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>86707.112521339062</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>64099.551779437606</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>64099.551779437606</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>132000</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>70.252955423154276</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>170</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="N11">
         <v>0</v>
       </c>
       <c r="O11">
-        <v>112.44956333535953</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>3.8373524836394758E-2</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <v>3.9293986534976552E-2</v>
+        <v>0</v>
       </c>
       <c r="R11">
-        <v>6.9721122291983759</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
add outage calculating process
</commit_message>
<xml_diff>
--- a/Delay Model/data.xlsx
+++ b/Delay Model/data.xlsx
@@ -386,34 +386,34 @@
         <v>0</v>
       </c>
       <c r="C1">
-        <v>597.76666610869222</v>
+        <v>306.50408290847901</v>
       </c>
       <c r="D1">
-        <v>597.76666610869222</v>
+        <v>306.50408290847901</v>
       </c>
       <c r="E1">
-        <v>597.76666610869222</v>
+        <v>306.50408290847901</v>
       </c>
       <c r="F1">
-        <v>597.76666610869222</v>
+        <v>306.50408290848014</v>
       </c>
       <c r="G1">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="H1">
         <v>0</v>
       </c>
       <c r="I1">
-        <v>15.00925925925926</v>
+        <v>15.044217687074831</v>
       </c>
       <c r="J1">
-        <v>15.00925925925926</v>
+        <v>15.044217687074831</v>
       </c>
       <c r="K1">
-        <v>15.00925925925926</v>
+        <v>15.044217687074831</v>
       </c>
       <c r="L1">
-        <v>15.00925925925926</v>
+        <v>15.044217687074729</v>
       </c>
       <c r="M1">
         <v>20</v>
@@ -422,16 +422,16 @@
         <v>0</v>
       </c>
       <c r="O1">
-        <v>1.5408032362923494</v>
+        <v>18.481891713230183</v>
       </c>
       <c r="P1">
-        <v>4.291125227128695E-3</v>
+        <v>5.359497648784229E-3</v>
       </c>
       <c r="Q1">
-        <v>4.8563158559438028E-3</v>
+        <v>5.6564573953785781E-3</v>
       </c>
       <c r="R1">
-        <v>1.1559243469445573E-2</v>
+        <v>2.5075241180238638E-3</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
@@ -442,34 +442,34 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1213.8314659213013</v>
+        <v>748.71154169204465</v>
       </c>
       <c r="D2">
-        <v>3098.6925920346184</v>
+        <v>2129.795400180607</v>
       </c>
       <c r="E2">
-        <v>1213.8314659213013</v>
+        <v>1914.6285076969839</v>
       </c>
       <c r="F2">
-        <v>1213.8314659213013</v>
+        <v>911.81207739129502</v>
       </c>
       <c r="G2">
-        <v>5500</v>
+        <v>5000</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>20.00925925925926</v>
+        <v>20.044217687074831</v>
       </c>
       <c r="J2">
-        <v>40.00925925925926</v>
+        <v>30</v>
       </c>
       <c r="K2">
-        <v>20.00925925925926</v>
+        <v>30</v>
       </c>
       <c r="L2">
-        <v>20.00925925925926</v>
+        <v>20.049259636141919</v>
       </c>
       <c r="M2">
         <v>25</v>
@@ -478,16 +478,16 @@
         <v>0</v>
       </c>
       <c r="O2">
-        <v>12.496017781175938</v>
+        <v>24.795251659163029</v>
       </c>
       <c r="P2">
-        <v>8.2127574362247657E-3</v>
+        <v>9.5018585584140305E-3</v>
       </c>
       <c r="Q2">
-        <v>9.400027534198727E-3</v>
+        <v>9.3371653656188873E-3</v>
       </c>
       <c r="R2">
-        <v>1.7778900384227227E-2</v>
+        <v>2.9640269106970363E-3</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -498,34 +498,34 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>1831.0968058474652</v>
+        <v>1423.7622406159676</v>
       </c>
       <c r="D3">
-        <v>5697.9344124444942</v>
+        <v>5129.7954001806065</v>
       </c>
       <c r="E3">
-        <v>3312.7986721435482</v>
+        <v>2585.5359637645511</v>
       </c>
       <c r="F3">
-        <v>1853.4138317015231</v>
+        <v>1604.0879345672024</v>
       </c>
       <c r="G3">
-        <v>8500</v>
+        <v>8000</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>25.069505850903518</v>
+        <v>25.044217687074831</v>
       </c>
       <c r="J3">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="K3">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="L3">
-        <v>25.02183501462946</v>
+        <v>25.054231228411776</v>
       </c>
       <c r="M3">
         <v>30</v>
@@ -534,16 +534,16 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>10.812115502550327</v>
+        <v>33.439194931886995</v>
       </c>
       <c r="P3">
-        <v>1.1727065548459622E-2</v>
+        <v>1.2132398535908804E-2</v>
       </c>
       <c r="Q3">
-        <v>1.2421393844855031E-2</v>
+        <v>1.2734566910947346E-2</v>
       </c>
       <c r="R3">
-        <v>1.4140859044244726E-2</v>
+        <v>5.2973019329690179E-3</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -554,34 +554,34 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>2437.2171318657583</v>
+        <v>2140.223972604711</v>
       </c>
       <c r="D4">
-        <v>6354.4662857630283</v>
+        <v>5869.7675198705365</v>
       </c>
       <c r="E4">
-        <v>3930.9541007312246</v>
+        <v>3325.5080834544806</v>
       </c>
       <c r="F4">
-        <v>2472.7581905799711</v>
+        <v>2354.4243853174103</v>
       </c>
       <c r="G4">
-        <v>11500</v>
+        <v>11000</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>31.002788310930264</v>
+        <v>30.044217687074831</v>
       </c>
       <c r="J4">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="K4">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="L4">
-        <v>30.02183501462946</v>
+        <v>30.066287547394531</v>
       </c>
       <c r="M4">
         <v>35</v>
@@ -590,16 +590,16 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <v>11.634779902765594</v>
+        <v>51.454941194005734</v>
       </c>
       <c r="P4">
-        <v>1.6023595215420971E-2</v>
+        <v>2.9356348282582798E-2</v>
       </c>
       <c r="Q4">
-        <v>1.6244323915954702E-2</v>
+        <v>3.0817822591013611E-2</v>
       </c>
       <c r="R4">
-        <v>2.1926665733689683E-2</v>
+        <v>7.7927192524351267E-3</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
@@ -610,34 +610,34 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>3048.1626989251881</v>
+        <v>2717.1177608244061</v>
       </c>
       <c r="D5">
-        <v>9354.4662857630283</v>
+        <v>6433.7129346635647</v>
       </c>
       <c r="E5">
-        <v>4547.7147772742701</v>
+        <v>3889.4534982475088</v>
       </c>
       <c r="F5">
-        <v>3090.3289270581863</v>
+        <v>2960.9831667057238</v>
       </c>
       <c r="G5">
-        <v>14500</v>
+        <v>14000</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>35.069505850903511</v>
+        <v>35.044217687074834</v>
       </c>
       <c r="J5">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="K5">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="L5">
-        <v>36.002788310930264</v>
+        <v>35.069828928961428</v>
       </c>
       <c r="M5">
         <v>40</v>
@@ -646,16 +646,16 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>13.76366327722956</v>
+        <v>61.567998946418676</v>
       </c>
       <c r="P5">
-        <v>2.1713048138198923E-2</v>
+        <v>2.0373884836507161E-2</v>
       </c>
       <c r="Q5">
-        <v>1.9913369673924545E-2</v>
+        <v>2.0351698188773103E-2</v>
       </c>
       <c r="R5">
-        <v>2.4592761236399301E-2</v>
+        <v>1.0642245140839701E-2</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
@@ -666,34 +666,34 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>3666.307839312406</v>
+        <v>3207.5564041495486</v>
       </c>
       <c r="D6">
-        <v>12354.466285763028</v>
+        <v>6924.1515779887068</v>
       </c>
       <c r="E6">
-        <v>5165.7702798778246</v>
+        <v>4379.8921415726509</v>
       </c>
       <c r="F6">
-        <v>3768.2711468801372</v>
+        <v>3503.3690674977679</v>
       </c>
       <c r="G6">
-        <v>17500</v>
+        <v>17000</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>40.069505850903511</v>
+        <v>40.044217687074834</v>
       </c>
       <c r="J6">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="K6">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="L6">
-        <v>40.336128811583919</v>
+        <v>40.072527122558661</v>
       </c>
       <c r="M6">
         <v>45</v>
@@ -702,16 +702,16 @@
         <v>0</v>
       </c>
       <c r="O6">
-        <v>12.819705896073192</v>
+        <v>36.736340704989267</v>
       </c>
       <c r="P6">
-        <v>2.4382556971329163E-2</v>
+        <v>2.640979079697852E-2</v>
       </c>
       <c r="Q6">
-        <v>2.4644814525313828E-2</v>
+        <v>2.7914216179868862E-2</v>
       </c>
       <c r="R6">
-        <v>4.0480107679197005E-2</v>
+        <v>1.5177203902119336E-2</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
@@ -722,34 +722,34 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>4286.9690472345419</v>
+        <v>3826.5315741711356</v>
       </c>
       <c r="D7">
-        <v>15354.466285763028</v>
+        <v>7543.1267480102942</v>
       </c>
       <c r="E7">
-        <v>5787.0770443659949</v>
+        <v>4995.7402857209872</v>
       </c>
       <c r="F7">
-        <v>4398.2862917699158</v>
+        <v>4168.8188419005755</v>
       </c>
       <c r="G7">
-        <v>20500</v>
+        <v>20000</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>46.002874884491249</v>
+        <v>45.044217687074827</v>
       </c>
       <c r="J7">
-        <v>145</v>
+        <v>65</v>
       </c>
       <c r="K7">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="L7">
-        <v>45.252799074315213</v>
+        <v>45.074852003245766</v>
       </c>
       <c r="M7">
         <v>50</v>
@@ -758,16 +758,16 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>32.385090231389668</v>
+        <v>71.583105209083556</v>
       </c>
       <c r="P7">
-        <v>2.6646732817010219E-2</v>
+        <v>2.683617265535489E-2</v>
       </c>
       <c r="Q7">
-        <v>2.7966269468783386E-2</v>
+        <v>2.7542732052424204E-2</v>
       </c>
       <c r="R7">
-        <v>7.477582952462547E-2</v>
+        <v>2.1834861652029167E-2</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
@@ -778,34 +778,34 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>4926.6813744271049</v>
+        <v>4447.7164724006834</v>
       </c>
       <c r="D8">
-        <v>18354.466285763028</v>
+        <v>8184.9283287885537</v>
       </c>
       <c r="E8">
-        <v>6406.4214032444424</v>
+        <v>5619.3862321498691</v>
       </c>
       <c r="F8">
-        <v>5026.7512794016639</v>
+        <v>4868.3692482874394</v>
       </c>
       <c r="G8">
-        <v>23500</v>
+        <v>23000</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>51.002874884491249</v>
+        <v>50.044217687074827</v>
       </c>
       <c r="J8">
-        <v>170</v>
+        <v>70</v>
       </c>
       <c r="K8">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="L8">
-        <v>50.145667055271574</v>
+        <v>50.08073183755355</v>
       </c>
       <c r="M8">
         <v>55</v>
@@ -814,16 +814,16 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>41.898456833316835</v>
+        <v>173.50511572896792</v>
       </c>
       <c r="P8">
-        <v>2.8650357773916921E-2</v>
+        <v>3.9251593171973825E-2</v>
       </c>
       <c r="Q8">
-        <v>2.9517059256553881E-2</v>
+        <v>3.3056967346943418E-2</v>
       </c>
       <c r="R8">
-        <v>6.0917139128485724E-2</v>
+        <v>4.7227585228016157E-2</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
@@ -834,34 +834,34 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>5583.44679105656</v>
+        <v>4743.8792325366303</v>
       </c>
       <c r="D9">
-        <v>21354.466285763028</v>
+        <v>8481.0910889245006</v>
       </c>
       <c r="E9">
-        <v>7026.9211703270275</v>
+        <v>5915.548992285816</v>
       </c>
       <c r="F9">
-        <v>5701.5529060626186</v>
+        <v>5283.543671113066</v>
       </c>
       <c r="G9">
-        <v>26500</v>
+        <v>26000</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>56.002874884491249</v>
+        <v>55.052403846153844</v>
       </c>
       <c r="J9">
-        <v>195</v>
+        <v>75</v>
       </c>
       <c r="K9">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="L9">
-        <v>55.093284387821207</v>
+        <v>55.081660485062379</v>
       </c>
       <c r="M9">
         <v>60</v>
@@ -870,16 +870,16 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>784.25220614922853</v>
+        <v>198.47734032155847</v>
       </c>
       <c r="P9">
-        <v>3.0473645106933952E-2</v>
+        <v>3.7620305675116934E-2</v>
       </c>
       <c r="Q9">
-        <v>3.2757163158331881E-2</v>
+        <v>4.3703429373073602E-2</v>
       </c>
       <c r="R9">
-        <v>0.18171234271657866</v>
+        <v>0.12199893617868557</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
@@ -890,34 +890,34 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>6145.8413918639462</v>
+        <v>5324.0519372706467</v>
       </c>
       <c r="D10">
-        <v>22357.117835452584</v>
+        <v>11481.091088924501</v>
       </c>
       <c r="E10">
-        <v>7680.2126479026692</v>
+        <v>6485.1725979249213</v>
       </c>
       <c r="F10">
-        <v>6351.0003111336837</v>
+        <v>5957.3234459801306</v>
       </c>
       <c r="G10">
-        <v>29500</v>
+        <v>29000</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>60.024021102492959</v>
+        <v>60.015890724937918</v>
       </c>
       <c r="J10">
-        <v>200.02651549689557</v>
+        <v>90</v>
       </c>
       <c r="K10">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="L10">
-        <v>60.021161769784591</v>
+        <v>60.03480390112599</v>
       </c>
       <c r="M10">
         <v>65</v>
@@ -926,301 +926,301 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>177.06416776746573</v>
+        <v>1125.1184610544688</v>
       </c>
       <c r="P10">
-        <v>3.4707312605315468E-2</v>
+        <v>3.804042976105549E-2</v>
       </c>
       <c r="Q10">
-        <v>3.5760893928481627E-2</v>
+        <v>3.5795027232687876E-2</v>
       </c>
       <c r="R10">
-        <v>5.8445603459751715E-2</v>
+        <v>9.8273851784090926E-2</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>5811.408529753634</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>14481.091088924501</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>7520.7655216721096</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>6878.6636113148788</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>32000</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>65.012284935195325</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>65.966991355439802</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="N11">
         <v>0</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>2354.4699382300973</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>3.8662793674416066E-2</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>3.8940980103696982E-2</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>0.30359976396820137</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>6344.5945747687656</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>17722.779321371192</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>8480.2491672083997</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>8076.8521740019578</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>70.012284935195325</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>75.649238649397986</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>3685.2387143918527</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>4.7465772829207185E-2</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>4.8170625561066188E-2</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>0.54541890410475746</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>7067.6327411904213</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>18445.81748779285</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>9203.2873336300545</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>9101.529322978311</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>38000</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>75.012284935195325</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>83.718637537139458</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="N13">
         <v>0</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>306.63783796237828</v>
       </c>
       <c r="P13">
-        <v>0</v>
+        <v>4.6577738031441322E-2</v>
       </c>
       <c r="Q13">
-        <v>0</v>
+        <v>4.7711248175290447E-2</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>0.61472545246539168</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>8240.6378593561785</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>21843.723122207048</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>9995.7996752080726</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>9989.5130500311716</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>41000</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>80.055576366532222</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>89.910630282508734</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>7200.8351617406615</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>5.2182995470510529E-2</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>5.0872845477394082E-2</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>0.38322450014620429</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>8513.208248724226</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>22262.922557139158</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>10413.075965441163</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>10413.075965441165</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>44000</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>85.114016693392543</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="N15">
         <v>0</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>7200.219314728407</v>
       </c>
       <c r="P15">
-        <v>0</v>
+        <v>5.6167205403984719E-2</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>5.5471739330782435E-2</v>
       </c>
       <c r="R15">
-        <v>0</v>
+        <v>0.37917724287097498</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1276,7 +1276,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1332,7 +1332,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1388,7 +1388,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>0</v>

</xml_diff>